<commit_message>
Atualização do banco e dos requisitos
</commit_message>
<xml_diff>
--- a/documentação/backlogs/backlogRequisitos.xlsx
+++ b/documentação/backlogs/backlogRequisitos.xlsx
@@ -1,11 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="28908"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="23127"/>
   <workbookPr/>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{272928C9-4965-486C-B924-E456782FD958}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\projeto_Individual\documentação\backlogs\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{99EBB75B-748A-4906-9DD4-FFE3FB412FF7}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11760" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Planilha1" sheetId="1" r:id="rId1"/>
@@ -22,8 +27,6 @@
         <xcalcf:feature name="microsoft.com:FV"/>
         <xcalcf:feature name="microsoft.com:CNMTM"/>
         <xcalcf:feature name="microsoft.com:LET_WF"/>
-        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
-        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
       </xcalcf:calcFeatures>
     </ext>
   </extLst>
@@ -31,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="105" uniqueCount="70">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="97" uniqueCount="65">
   <si>
     <t>Backlog de Requisitos</t>
   </si>
@@ -108,9 +111,6 @@
     <t>Foto de Perfil</t>
   </si>
   <si>
-    <t>O sistema deve exibir o avatar padrão do usuário na barra lateral.</t>
-  </si>
-  <si>
     <t>RNF008</t>
   </si>
   <si>
@@ -118,18 +118,6 @@
   </si>
   <si>
     <t>O sistema deve exibir a biografia do usuário.</t>
-  </si>
-  <si>
-    <t>RNF009</t>
-  </si>
-  <si>
-    <t>Níumero de Seguidores(Perfil)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">	O sistema deve mostrar o número de seguidores do usuário.</t>
-  </si>
-  <si>
-    <t>RNF010</t>
   </si>
   <si>
     <t>Botão Dashboard</t>
@@ -329,8 +317,8 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{474880A3-481C-4969-83C7-C0E995508586}" name="Tabela1" displayName="Tabela1" ref="B2:E27" totalsRowShown="0" dataDxfId="4">
-  <autoFilter ref="B2:E27" xr:uid="{474880A3-481C-4969-83C7-C0E995508586}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{474880A3-481C-4969-83C7-C0E995508586}" name="Tabela1" displayName="Tabela1" ref="B2:E25" totalsRowShown="0" dataDxfId="4">
+  <autoFilter ref="B2:E25" xr:uid="{474880A3-481C-4969-83C7-C0E995508586}"/>
   <tableColumns count="4">
     <tableColumn id="4" xr3:uid="{3FC0F141-40B2-43D0-9D46-AD591C5862D6}" name="Tipo" dataDxfId="3"/>
     <tableColumn id="1" xr3:uid="{381572D0-0C7E-4E6E-83B2-C50762865A46}" name="Código" dataDxfId="2"/>
@@ -658,21 +646,21 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:E37"/>
+  <dimension ref="A1:E35"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A25" workbookViewId="0">
-      <selection activeCell="C27" sqref="C27"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F10" sqref="F10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="14.25"/>
   <cols>
-    <col min="1" max="1" width="28.28515625" customWidth="1"/>
-    <col min="2" max="2" width="17.7109375" customWidth="1"/>
-    <col min="3" max="3" width="17.28515625" customWidth="1"/>
-    <col min="4" max="5" width="19.42578125" customWidth="1"/>
+    <col min="1" max="1" width="28.25" customWidth="1"/>
+    <col min="2" max="2" width="17.75" customWidth="1"/>
+    <col min="3" max="3" width="17.25" customWidth="1"/>
+    <col min="4" max="5" width="19.375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" ht="21">
+    <row r="1" spans="1:5" ht="20.25">
       <c r="A1" s="4" t="s">
         <v>0</v>
       </c>
@@ -691,7 +679,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="3" spans="1:5" ht="72.75">
+    <row r="3" spans="1:5" ht="71.25">
       <c r="B3" s="2" t="s">
         <v>5</v>
       </c>
@@ -705,7 +693,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="4" spans="1:5" ht="57.75">
+    <row r="4" spans="1:5" ht="42.75">
       <c r="B4" s="2" t="s">
         <v>5</v>
       </c>
@@ -719,7 +707,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="5" spans="1:5" ht="72.75">
+    <row r="5" spans="1:5" ht="71.25">
       <c r="B5" s="2" t="s">
         <v>5</v>
       </c>
@@ -733,7 +721,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="6" spans="1:5" ht="57.75">
+    <row r="6" spans="1:5" ht="42.75">
       <c r="B6" s="2" t="s">
         <v>5</v>
       </c>
@@ -747,7 +735,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="7" spans="1:5" ht="57.75">
+    <row r="7" spans="1:5" ht="42.75">
       <c r="B7" s="2" t="s">
         <v>5</v>
       </c>
@@ -761,7 +749,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="8" spans="1:5" ht="57.75">
+    <row r="8" spans="1:5" ht="57">
       <c r="B8" s="2" t="s">
         <v>5</v>
       </c>
@@ -775,7 +763,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="9" spans="1:5" ht="57.75">
+    <row r="9" spans="1:5" ht="28.5">
       <c r="B9" s="2" t="s">
         <v>5</v>
       </c>
@@ -783,263 +771,247 @@
         <v>23</v>
       </c>
       <c r="D9" s="3" t="s">
-        <v>24</v>
+        <v>26</v>
       </c>
       <c r="E9" s="1" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="10" spans="1:5" ht="29.25">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5" ht="57">
       <c r="B10" s="2" t="s">
         <v>5</v>
       </c>
       <c r="C10" s="2" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="D10" s="3" t="s">
-        <v>27</v>
-      </c>
-      <c r="E10" s="1" t="s">
         <v>28</v>
       </c>
-    </row>
-    <row r="11" spans="1:5" ht="72.75">
+      <c r="E10" s="3" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5" ht="71.25">
       <c r="B11" s="2" t="s">
-        <v>5</v>
+        <v>30</v>
       </c>
       <c r="C11" s="2" t="s">
-        <v>29</v>
+        <v>31</v>
       </c>
       <c r="D11" s="3" t="s">
-        <v>30</v>
+        <v>32</v>
       </c>
       <c r="E11" s="3" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="12" spans="1:5" ht="57.75">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="12" spans="1:5" ht="57">
       <c r="B12" s="2" t="s">
-        <v>5</v>
+        <v>30</v>
       </c>
       <c r="C12" s="2" t="s">
-        <v>32</v>
+        <v>34</v>
       </c>
       <c r="D12" s="3" t="s">
-        <v>33</v>
+        <v>35</v>
       </c>
       <c r="E12" s="3" t="s">
-        <v>34</v>
-      </c>
-    </row>
-    <row r="13" spans="1:5" ht="72.75">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="13" spans="1:5" ht="42.75">
       <c r="B13" s="2" t="s">
+        <v>30</v>
+      </c>
+      <c r="C13" s="2" t="s">
+        <v>37</v>
+      </c>
+      <c r="D13" s="3" t="s">
         <v>35</v>
-      </c>
-      <c r="C13" s="2" t="s">
-        <v>36</v>
-      </c>
-      <c r="D13" s="3" t="s">
-        <v>37</v>
       </c>
       <c r="E13" s="3" t="s">
         <v>38</v>
       </c>
     </row>
-    <row r="14" spans="1:5" ht="57.75">
+    <row r="14" spans="1:5" ht="57">
       <c r="B14" s="2" t="s">
-        <v>35</v>
+        <v>30</v>
       </c>
       <c r="C14" s="2" t="s">
         <v>39</v>
       </c>
       <c r="D14" s="3" t="s">
+        <v>35</v>
+      </c>
+      <c r="E14" s="3" t="s">
         <v>40</v>
       </c>
-      <c r="E14" s="3" t="s">
+    </row>
+    <row r="15" spans="1:5" ht="71.25">
+      <c r="B15" s="2" t="s">
+        <v>30</v>
+      </c>
+      <c r="C15" s="2" t="s">
         <v>41</v>
       </c>
-    </row>
-    <row r="15" spans="1:5" ht="43.5">
-      <c r="B15" s="2" t="s">
-        <v>35</v>
-      </c>
-      <c r="C15" s="2" t="s">
+      <c r="D15" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="E15" s="3" t="s">
         <v>42</v>
       </c>
-      <c r="D15" s="3" t="s">
-        <v>40</v>
-      </c>
-      <c r="E15" s="3" t="s">
+    </row>
+    <row r="16" spans="1:5" ht="42.75">
+      <c r="B16" s="2" t="s">
+        <v>30</v>
+      </c>
+      <c r="C16" s="2" t="s">
         <v>43</v>
       </c>
-    </row>
-    <row r="16" spans="1:5" ht="57.75">
-      <c r="B16" s="2" t="s">
-        <v>35</v>
-      </c>
-      <c r="C16" s="2" t="s">
+      <c r="D16" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="E16" s="3" t="s">
         <v>44</v>
       </c>
-      <c r="D16" s="3" t="s">
-        <v>40</v>
-      </c>
-      <c r="E16" s="3" t="s">
+    </row>
+    <row r="17" spans="2:5" ht="57">
+      <c r="B17" s="2" t="s">
+        <v>30</v>
+      </c>
+      <c r="C17" s="2" t="s">
         <v>45</v>
       </c>
-    </row>
-    <row r="17" spans="2:5" ht="72.75">
-      <c r="B17" s="2" t="s">
-        <v>35</v>
-      </c>
-      <c r="C17" s="2" t="s">
+      <c r="D17" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="E17" s="1" t="s">
         <v>46</v>
       </c>
-      <c r="D17" s="3" t="s">
-        <v>10</v>
-      </c>
-      <c r="E17" s="3" t="s">
+    </row>
+    <row r="18" spans="2:5" ht="42.75">
+      <c r="B18" s="2" t="s">
+        <v>30</v>
+      </c>
+      <c r="C18" s="2" t="s">
         <v>47</v>
       </c>
-    </row>
-    <row r="18" spans="2:5" ht="43.5">
-      <c r="B18" s="2" t="s">
-        <v>35</v>
-      </c>
-      <c r="C18" s="2" t="s">
+      <c r="D18" s="3" t="s">
+        <v>21</v>
+      </c>
+      <c r="E18" s="3" t="s">
         <v>48</v>
       </c>
-      <c r="D18" s="3" t="s">
-        <v>15</v>
-      </c>
-      <c r="E18" s="3" t="s">
+    </row>
+    <row r="19" spans="2:5" ht="42.75">
+      <c r="B19" s="2" t="s">
+        <v>30</v>
+      </c>
+      <c r="C19" s="2" t="s">
         <v>49</v>
       </c>
-    </row>
-    <row r="19" spans="2:5" ht="57.75">
-      <c r="B19" s="2" t="s">
-        <v>35</v>
-      </c>
-      <c r="C19" s="2" t="s">
+      <c r="D19" s="3" t="s">
+        <v>21</v>
+      </c>
+      <c r="E19" s="3" t="s">
         <v>50</v>
       </c>
-      <c r="D19" s="3" t="s">
-        <v>18</v>
-      </c>
-      <c r="E19" s="1" t="s">
+    </row>
+    <row r="20" spans="2:5" ht="57">
+      <c r="B20" s="2" t="s">
+        <v>30</v>
+      </c>
+      <c r="C20" s="2" t="s">
         <v>51</v>
       </c>
-    </row>
-    <row r="20" spans="2:5" ht="57.75">
-      <c r="B20" s="2" t="s">
-        <v>35</v>
-      </c>
-      <c r="C20" s="2" t="s">
+      <c r="D20" s="3" t="s">
+        <v>24</v>
+      </c>
+      <c r="E20" s="3" t="s">
         <v>52</v>
       </c>
-      <c r="D20" s="3" t="s">
-        <v>21</v>
-      </c>
-      <c r="E20" s="3" t="s">
+    </row>
+    <row r="21" spans="2:5" ht="71.25">
+      <c r="B21" s="2" t="s">
+        <v>30</v>
+      </c>
+      <c r="C21" s="2" t="s">
         <v>53</v>
       </c>
-    </row>
-    <row r="21" spans="2:5" ht="43.5">
-      <c r="B21" s="2" t="s">
-        <v>35</v>
-      </c>
-      <c r="C21" s="2" t="s">
+      <c r="D21" s="3" t="s">
+        <v>24</v>
+      </c>
+      <c r="E21" s="3" t="s">
         <v>54</v>
       </c>
-      <c r="D21" s="3" t="s">
-        <v>21</v>
-      </c>
-      <c r="E21" s="3" t="s">
+    </row>
+    <row r="22" spans="2:5" ht="42.75">
+      <c r="B22" s="2" t="s">
+        <v>30</v>
+      </c>
+      <c r="C22" s="2" t="s">
         <v>55</v>
       </c>
-    </row>
-    <row r="22" spans="2:5" ht="57.75">
-      <c r="B22" s="2" t="s">
-        <v>35</v>
-      </c>
-      <c r="C22" s="2" t="s">
+      <c r="D22" s="3" t="s">
         <v>56</v>
-      </c>
-      <c r="D22" s="3" t="s">
-        <v>24</v>
       </c>
       <c r="E22" s="3" t="s">
         <v>57</v>
       </c>
     </row>
-    <row r="23" spans="2:5" ht="72.75">
+    <row r="23" spans="2:5" ht="85.5">
       <c r="B23" s="2" t="s">
-        <v>35</v>
+        <v>30</v>
       </c>
       <c r="C23" s="2" t="s">
         <v>58</v>
       </c>
       <c r="D23" s="3" t="s">
-        <v>24</v>
+        <v>59</v>
       </c>
       <c r="E23" s="3" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="24" spans="2:5" ht="57">
+      <c r="B24" s="2" t="s">
+        <v>30</v>
+      </c>
+      <c r="C24" s="2" t="s">
+        <v>61</v>
+      </c>
+      <c r="D24" s="3" t="s">
         <v>59</v>
-      </c>
-    </row>
-    <row r="24" spans="2:5" ht="43.5">
-      <c r="B24" s="2" t="s">
-        <v>35</v>
-      </c>
-      <c r="C24" s="2" t="s">
-        <v>60</v>
-      </c>
-      <c r="D24" s="3" t="s">
-        <v>61</v>
       </c>
       <c r="E24" s="3" t="s">
         <v>62</v>
       </c>
     </row>
-    <row r="25" spans="2:5" ht="87">
+    <row r="25" spans="2:5" ht="42.75">
       <c r="B25" s="2" t="s">
-        <v>35</v>
+        <v>30</v>
       </c>
       <c r="C25" s="2" t="s">
         <v>63</v>
       </c>
       <c r="D25" s="3" t="s">
+        <v>59</v>
+      </c>
+      <c r="E25" s="3" t="s">
         <v>64</v>
       </c>
-      <c r="E25" s="3" t="s">
-        <v>65</v>
-      </c>
-    </row>
-    <row r="26" spans="2:5" ht="57.75">
-      <c r="B26" s="2" t="s">
-        <v>35</v>
-      </c>
-      <c r="C26" s="2" t="s">
-        <v>66</v>
-      </c>
-      <c r="D26" s="3" t="s">
-        <v>64</v>
-      </c>
-      <c r="E26" s="3" t="s">
-        <v>67</v>
-      </c>
-    </row>
-    <row r="27" spans="2:5" ht="57.75">
-      <c r="B27" s="2" t="s">
-        <v>35</v>
-      </c>
-      <c r="C27" s="2" t="s">
-        <v>68</v>
-      </c>
-      <c r="D27" s="3" t="s">
-        <v>64</v>
-      </c>
-      <c r="E27" s="3" t="s">
-        <v>69</v>
-      </c>
+    </row>
+    <row r="26" spans="2:5">
+      <c r="B26" s="2"/>
+      <c r="C26" s="2"/>
+      <c r="D26" s="3"/>
+      <c r="E26" s="3"/>
+    </row>
+    <row r="27" spans="2:5">
+      <c r="B27" s="2"/>
+      <c r="C27" s="2"/>
+      <c r="D27" s="3"/>
+      <c r="E27" s="3"/>
     </row>
     <row r="28" spans="2:5">
       <c r="B28" s="2"/>
@@ -1088,18 +1060,6 @@
       <c r="C35" s="2"/>
       <c r="D35" s="3"/>
       <c r="E35" s="3"/>
-    </row>
-    <row r="36" spans="2:5">
-      <c r="B36" s="2"/>
-      <c r="C36" s="2"/>
-      <c r="D36" s="3"/>
-      <c r="E36" s="3"/>
-    </row>
-    <row r="37" spans="2:5">
-      <c r="B37" s="2"/>
-      <c r="C37" s="2"/>
-      <c r="D37" s="3"/>
-      <c r="E37" s="3"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
Backlogs e documentação com novas versões
</commit_message>
<xml_diff>
--- a/documentação/backlogs/backlogRequisitos.xlsx
+++ b/documentação/backlogs/backlogRequisitos.xlsx
@@ -1,16 +1,11 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="23127"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="28928"/>
   <workbookPr/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\projeto_Individual\documentação\backlogs\"/>
-    </mc:Choice>
-  </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{99EBB75B-748A-4906-9DD4-FFE3FB412FF7}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{52334238-B8DA-4A82-92D0-9AA6AC3FA863}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11760" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Planilha1" sheetId="1" r:id="rId1"/>
@@ -27,6 +22,8 @@
         <xcalcf:feature name="microsoft.com:FV"/>
         <xcalcf:feature name="microsoft.com:CNMTM"/>
         <xcalcf:feature name="microsoft.com:LET_WF"/>
+        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
+        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
       </xcalcf:calcFeatures>
     </ext>
   </extLst>
@@ -34,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="97" uniqueCount="65">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="89" uniqueCount="59">
   <si>
     <t>Backlog de Requisitos</t>
   </si>
@@ -111,15 +108,12 @@
     <t>Foto de Perfil</t>
   </si>
   <si>
+    <t>O sistema deve exibir o avatar padrão do usuário na barra lateral.</t>
+  </si>
+  <si>
     <t>RNF008</t>
   </si>
   <si>
-    <t>Biografia(Perfil)</t>
-  </si>
-  <si>
-    <t>O sistema deve exibir a biografia do usuário.</t>
-  </si>
-  <si>
     <t>Botão Dashboard</t>
   </si>
   <si>
@@ -204,31 +198,16 @@
     <t>RF012</t>
   </si>
   <si>
-    <t>Perfil</t>
-  </si>
-  <si>
-    <t>O sistema deve listar todos os posts feitos pelo usuário.</t>
+    <t>Dashboard</t>
+  </si>
+  <si>
+    <t>O sistema deve exibir estatísticas como número de posts, curtidas e comentários recebidos.</t>
   </si>
   <si>
     <t>RF013</t>
   </si>
   <si>
-    <t>Dashboard</t>
-  </si>
-  <si>
-    <t>O sistema deve exibir estatísticas como número de posts, curtidas e comentários recebidos.</t>
-  </si>
-  <si>
-    <t>RF014</t>
-  </si>
-  <si>
     <t>O sistema deve exibir gráficos simples com engajamento ao longo do tempo.</t>
-  </si>
-  <si>
-    <t>RF015</t>
-  </si>
-  <si>
-    <t xml:space="preserve">	O sistema deve sugerir ações com base nas métricas.</t>
   </si>
 </sst>
 </file>
@@ -317,8 +296,8 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{474880A3-481C-4969-83C7-C0E995508586}" name="Tabela1" displayName="Tabela1" ref="B2:E25" totalsRowShown="0" dataDxfId="4">
-  <autoFilter ref="B2:E25" xr:uid="{474880A3-481C-4969-83C7-C0E995508586}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{474880A3-481C-4969-83C7-C0E995508586}" name="Tabela1" displayName="Tabela1" ref="B2:E23" totalsRowShown="0" dataDxfId="4">
+  <autoFilter ref="B2:E23" xr:uid="{474880A3-481C-4969-83C7-C0E995508586}"/>
   <tableColumns count="4">
     <tableColumn id="4" xr3:uid="{3FC0F141-40B2-43D0-9D46-AD591C5862D6}" name="Tipo" dataDxfId="3"/>
     <tableColumn id="1" xr3:uid="{381572D0-0C7E-4E6E-83B2-C50762865A46}" name="Código" dataDxfId="2"/>
@@ -646,21 +625,21 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:E35"/>
+  <dimension ref="A1:E33"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F10" sqref="F10"/>
+    <sheetView tabSelected="1" topLeftCell="A20" workbookViewId="0">
+      <selection activeCell="F23" sqref="F23"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.25"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="28.25" customWidth="1"/>
-    <col min="2" max="2" width="17.75" customWidth="1"/>
-    <col min="3" max="3" width="17.25" customWidth="1"/>
-    <col min="4" max="5" width="19.375" customWidth="1"/>
+    <col min="1" max="1" width="28.28515625" customWidth="1"/>
+    <col min="2" max="2" width="17.7109375" customWidth="1"/>
+    <col min="3" max="3" width="17.28515625" customWidth="1"/>
+    <col min="4" max="5" width="19.42578125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" ht="20.25">
+    <row r="1" spans="1:5" ht="21">
       <c r="A1" s="4" t="s">
         <v>0</v>
       </c>
@@ -679,7 +658,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="3" spans="1:5" ht="71.25">
+    <row r="3" spans="1:5" ht="72.75">
       <c r="B3" s="2" t="s">
         <v>5</v>
       </c>
@@ -693,7 +672,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="4" spans="1:5" ht="42.75">
+    <row r="4" spans="1:5" ht="57.75">
       <c r="B4" s="2" t="s">
         <v>5</v>
       </c>
@@ -707,7 +686,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="5" spans="1:5" ht="71.25">
+    <row r="5" spans="1:5" ht="72.75">
       <c r="B5" s="2" t="s">
         <v>5</v>
       </c>
@@ -721,7 +700,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="6" spans="1:5" ht="42.75">
+    <row r="6" spans="1:5" ht="57.75">
       <c r="B6" s="2" t="s">
         <v>5</v>
       </c>
@@ -735,7 +714,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="7" spans="1:5" ht="42.75">
+    <row r="7" spans="1:5" ht="57.75">
       <c r="B7" s="2" t="s">
         <v>5</v>
       </c>
@@ -749,7 +728,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="8" spans="1:5" ht="57">
+    <row r="8" spans="1:5" ht="57.75">
       <c r="B8" s="2" t="s">
         <v>5</v>
       </c>
@@ -763,7 +742,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="9" spans="1:5" ht="28.5">
+    <row r="9" spans="1:5" ht="57.75">
       <c r="B9" s="2" t="s">
         <v>5</v>
       </c>
@@ -771,235 +750,219 @@
         <v>23</v>
       </c>
       <c r="D9" s="3" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="E9" s="1" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="10" spans="1:5" ht="57">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5" ht="57.75">
       <c r="B10" s="2" t="s">
         <v>5</v>
       </c>
       <c r="C10" s="2" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="D10" s="3" t="s">
+        <v>27</v>
+      </c>
+      <c r="E10" s="3" t="s">
         <v>28</v>
       </c>
-      <c r="E10" s="3" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="11" spans="1:5" ht="71.25">
+    </row>
+    <row r="11" spans="1:5" ht="72.75">
       <c r="B11" s="2" t="s">
+        <v>29</v>
+      </c>
+      <c r="C11" s="2" t="s">
         <v>30</v>
       </c>
-      <c r="C11" s="2" t="s">
+      <c r="D11" s="3" t="s">
         <v>31</v>
       </c>
-      <c r="D11" s="3" t="s">
+      <c r="E11" s="3" t="s">
         <v>32</v>
       </c>
-      <c r="E11" s="3" t="s">
+    </row>
+    <row r="12" spans="1:5" ht="57.75">
+      <c r="B12" s="2" t="s">
+        <v>29</v>
+      </c>
+      <c r="C12" s="2" t="s">
         <v>33</v>
       </c>
-    </row>
-    <row r="12" spans="1:5" ht="57">
-      <c r="B12" s="2" t="s">
-        <v>30</v>
-      </c>
-      <c r="C12" s="2" t="s">
+      <c r="D12" s="3" t="s">
         <v>34</v>
       </c>
-      <c r="D12" s="3" t="s">
+      <c r="E12" s="3" t="s">
         <v>35</v>
       </c>
-      <c r="E12" s="3" t="s">
+    </row>
+    <row r="13" spans="1:5" ht="43.5">
+      <c r="B13" s="2" t="s">
+        <v>29</v>
+      </c>
+      <c r="C13" s="2" t="s">
         <v>36</v>
       </c>
-    </row>
-    <row r="13" spans="1:5" ht="42.75">
-      <c r="B13" s="2" t="s">
-        <v>30</v>
-      </c>
-      <c r="C13" s="2" t="s">
+      <c r="D13" s="3" t="s">
+        <v>34</v>
+      </c>
+      <c r="E13" s="3" t="s">
         <v>37</v>
       </c>
-      <c r="D13" s="3" t="s">
-        <v>35</v>
-      </c>
-      <c r="E13" s="3" t="s">
+    </row>
+    <row r="14" spans="1:5" ht="57.75">
+      <c r="B14" s="2" t="s">
+        <v>29</v>
+      </c>
+      <c r="C14" s="2" t="s">
         <v>38</v>
       </c>
-    </row>
-    <row r="14" spans="1:5" ht="57">
-      <c r="B14" s="2" t="s">
-        <v>30</v>
-      </c>
-      <c r="C14" s="2" t="s">
+      <c r="D14" s="3" t="s">
+        <v>34</v>
+      </c>
+      <c r="E14" s="3" t="s">
         <v>39</v>
       </c>
-      <c r="D14" s="3" t="s">
-        <v>35</v>
-      </c>
-      <c r="E14" s="3" t="s">
+    </row>
+    <row r="15" spans="1:5" ht="72.75">
+      <c r="B15" s="2" t="s">
+        <v>29</v>
+      </c>
+      <c r="C15" s="2" t="s">
         <v>40</v>
-      </c>
-    </row>
-    <row r="15" spans="1:5" ht="71.25">
-      <c r="B15" s="2" t="s">
-        <v>30</v>
-      </c>
-      <c r="C15" s="2" t="s">
-        <v>41</v>
       </c>
       <c r="D15" s="3" t="s">
         <v>10</v>
       </c>
       <c r="E15" s="3" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="16" spans="1:5" ht="43.5">
+      <c r="B16" s="2" t="s">
+        <v>29</v>
+      </c>
+      <c r="C16" s="2" t="s">
         <v>42</v>
-      </c>
-    </row>
-    <row r="16" spans="1:5" ht="42.75">
-      <c r="B16" s="2" t="s">
-        <v>30</v>
-      </c>
-      <c r="C16" s="2" t="s">
-        <v>43</v>
       </c>
       <c r="D16" s="3" t="s">
         <v>15</v>
       </c>
       <c r="E16" s="3" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="17" spans="2:5" ht="57.75">
+      <c r="B17" s="2" t="s">
+        <v>29</v>
+      </c>
+      <c r="C17" s="2" t="s">
         <v>44</v>
-      </c>
-    </row>
-    <row r="17" spans="2:5" ht="57">
-      <c r="B17" s="2" t="s">
-        <v>30</v>
-      </c>
-      <c r="C17" s="2" t="s">
-        <v>45</v>
       </c>
       <c r="D17" s="3" t="s">
         <v>18</v>
       </c>
       <c r="E17" s="1" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="18" spans="2:5" ht="57.75">
+      <c r="B18" s="2" t="s">
+        <v>29</v>
+      </c>
+      <c r="C18" s="2" t="s">
         <v>46</v>
-      </c>
-    </row>
-    <row r="18" spans="2:5" ht="42.75">
-      <c r="B18" s="2" t="s">
-        <v>30</v>
-      </c>
-      <c r="C18" s="2" t="s">
-        <v>47</v>
       </c>
       <c r="D18" s="3" t="s">
         <v>21</v>
       </c>
       <c r="E18" s="3" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="19" spans="2:5" ht="43.5">
+      <c r="B19" s="2" t="s">
+        <v>29</v>
+      </c>
+      <c r="C19" s="2" t="s">
         <v>48</v>
-      </c>
-    </row>
-    <row r="19" spans="2:5" ht="42.75">
-      <c r="B19" s="2" t="s">
-        <v>30</v>
-      </c>
-      <c r="C19" s="2" t="s">
-        <v>49</v>
       </c>
       <c r="D19" s="3" t="s">
         <v>21</v>
       </c>
       <c r="E19" s="3" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="20" spans="2:5" ht="57.75">
+      <c r="B20" s="2" t="s">
+        <v>29</v>
+      </c>
+      <c r="C20" s="2" t="s">
         <v>50</v>
-      </c>
-    </row>
-    <row r="20" spans="2:5" ht="57">
-      <c r="B20" s="2" t="s">
-        <v>30</v>
-      </c>
-      <c r="C20" s="2" t="s">
-        <v>51</v>
       </c>
       <c r="D20" s="3" t="s">
         <v>24</v>
       </c>
       <c r="E20" s="3" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="21" spans="2:5" ht="72.75">
+      <c r="B21" s="2" t="s">
+        <v>29</v>
+      </c>
+      <c r="C21" s="2" t="s">
         <v>52</v>
-      </c>
-    </row>
-    <row r="21" spans="2:5" ht="71.25">
-      <c r="B21" s="2" t="s">
-        <v>30</v>
-      </c>
-      <c r="C21" s="2" t="s">
-        <v>53</v>
       </c>
       <c r="D21" s="3" t="s">
         <v>24</v>
       </c>
       <c r="E21" s="3" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="22" spans="2:5" ht="87">
+      <c r="B22" s="2" t="s">
+        <v>29</v>
+      </c>
+      <c r="C22" s="2" t="s">
         <v>54</v>
       </c>
-    </row>
-    <row r="22" spans="2:5" ht="42.75">
-      <c r="B22" s="2" t="s">
-        <v>30</v>
-      </c>
-      <c r="C22" s="2" t="s">
+      <c r="D22" s="3" t="s">
         <v>55</v>
       </c>
-      <c r="D22" s="3" t="s">
+      <c r="E22" s="3" t="s">
         <v>56</v>
       </c>
-      <c r="E22" s="3" t="s">
+    </row>
+    <row r="23" spans="2:5" ht="57.75">
+      <c r="B23" s="2" t="s">
+        <v>29</v>
+      </c>
+      <c r="C23" s="2" t="s">
         <v>57</v>
       </c>
-    </row>
-    <row r="23" spans="2:5" ht="85.5">
-      <c r="B23" s="2" t="s">
-        <v>30</v>
-      </c>
-      <c r="C23" s="2" t="s">
+      <c r="D23" s="3" t="s">
+        <v>55</v>
+      </c>
+      <c r="E23" s="3" t="s">
         <v>58</v>
       </c>
-      <c r="D23" s="3" t="s">
-        <v>59</v>
-      </c>
-      <c r="E23" s="3" t="s">
-        <v>60</v>
-      </c>
-    </row>
-    <row r="24" spans="2:5" ht="57">
-      <c r="B24" s="2" t="s">
-        <v>30</v>
-      </c>
-      <c r="C24" s="2" t="s">
-        <v>61</v>
-      </c>
-      <c r="D24" s="3" t="s">
-        <v>59</v>
-      </c>
-      <c r="E24" s="3" t="s">
-        <v>62</v>
-      </c>
-    </row>
-    <row r="25" spans="2:5" ht="42.75">
-      <c r="B25" s="2" t="s">
-        <v>30</v>
-      </c>
-      <c r="C25" s="2" t="s">
-        <v>63</v>
-      </c>
-      <c r="D25" s="3" t="s">
-        <v>59</v>
-      </c>
-      <c r="E25" s="3" t="s">
-        <v>64</v>
-      </c>
+    </row>
+    <row r="24" spans="2:5">
+      <c r="B24" s="2"/>
+      <c r="C24" s="2"/>
+      <c r="D24" s="3"/>
+      <c r="E24" s="3"/>
+    </row>
+    <row r="25" spans="2:5">
+      <c r="B25" s="2"/>
+      <c r="C25" s="2"/>
+      <c r="D25" s="3"/>
+      <c r="E25" s="3"/>
     </row>
     <row r="26" spans="2:5">
       <c r="B26" s="2"/>
@@ -1048,18 +1011,6 @@
       <c r="C33" s="2"/>
       <c r="D33" s="3"/>
       <c r="E33" s="3"/>
-    </row>
-    <row r="34" spans="2:5">
-      <c r="B34" s="2"/>
-      <c r="C34" s="2"/>
-      <c r="D34" s="3"/>
-      <c r="E34" s="3"/>
-    </row>
-    <row r="35" spans="2:5">
-      <c r="B35" s="2"/>
-      <c r="C35" s="2"/>
-      <c r="D35" s="3"/>
-      <c r="E35" s="3"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>